<commit_message>
Blackified, final directory cleanup
</commit_message>
<xml_diff>
--- a/bouman_8.xlsx
+++ b/bouman_8.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kvnpo\Desktop\DataScience\BeCode\01-TheField\Projects\Project\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2433567-34FE-422A-9975-2057F27E036A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -25,98 +20,149 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
-  <si>
-    <t>Miro</t>
-  </si>
-  <si>
-    <t>Fatemeh</t>
-  </si>
-  <si>
-    <t>Mohamad</t>
-  </si>
-  <si>
-    <t>Celina</t>
-  </si>
-  <si>
-    <t>Aleksander</t>
-  </si>
-  <si>
-    <t>David</t>
-  </si>
-  <si>
-    <t>Miriam</t>
-  </si>
-  <si>
-    <t>Olha</t>
-  </si>
-  <si>
-    <t>An</t>
-  </si>
-  <si>
-    <t>Dhanya</t>
-  </si>
-  <si>
-    <t>Andrii</t>
-  </si>
-  <si>
-    <t>Therese</t>
-  </si>
-  <si>
-    <t>Edoardo</t>
-  </si>
-  <si>
-    <t>Oscar</t>
-  </si>
-  <si>
-    <t>Frank</t>
-  </si>
-  <si>
-    <t>Beatriz</t>
-  </si>
-  <si>
-    <t>Kevin J</t>
-  </si>
-  <si>
-    <t>Patrick</t>
-  </si>
-  <si>
-    <t>Manel</t>
-  </si>
-  <si>
-    <t>Jessica</t>
-  </si>
-  <si>
-    <t>Vera</t>
-  </si>
-  <si>
-    <t>Imad</t>
-  </si>
-  <si>
-    <t>Kevin P</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+  <si>
+    <t xml:space="preserve">Miro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fatemeh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mohamad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Celina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aleksander</t>
+  </si>
+  <si>
+    <t xml:space="preserve">David</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miriam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dhanya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andrii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Therese</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edoardo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oscar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beatriz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kevin J</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patrick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jessica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kevin P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patrycja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Karthika</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elsa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nicole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stef</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maxim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boitumelo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yassine</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="General"/>
+  </numFmts>
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -129,7 +175,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -137,81 +183,107 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4285F4"/>
+        <a:srgbClr val="4285f4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="EA4335"/>
+        <a:srgbClr val="ea4335"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="FBBC04"/>
+        <a:srgbClr val="fbbc04"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="34A853"/>
+        <a:srgbClr val="34a853"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="FF6D01"/>
+        <a:srgbClr val="ff6d01"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="46BDC6"/>
+        <a:srgbClr val="46bdc6"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="1155cc"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="1155cc"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Sheets">
       <a:majorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:cs typeface="Arial" pitchFamily="0" charset="1"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:cs typeface="Arial" pitchFamily="0" charset="1"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme>
@@ -241,7 +313,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -265,7 +337,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -325,173 +397,199 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:A33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:A33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="14" x14ac:dyDescent="0.3">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="14" x14ac:dyDescent="0.3">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="14" x14ac:dyDescent="0.3">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="14" x14ac:dyDescent="0.3">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="14" x14ac:dyDescent="0.3">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="14" x14ac:dyDescent="0.3">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="14" x14ac:dyDescent="0.3">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="14" x14ac:dyDescent="0.3">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="14" x14ac:dyDescent="0.3">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="14" x14ac:dyDescent="0.3">
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="14" x14ac:dyDescent="0.3">
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="14" x14ac:dyDescent="0.3">
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="14" x14ac:dyDescent="0.3">
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="14" x14ac:dyDescent="0.3">
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="14" x14ac:dyDescent="0.3">
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="14" x14ac:dyDescent="0.3">
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="14" x14ac:dyDescent="0.3">
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="14" x14ac:dyDescent="0.3">
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="14" x14ac:dyDescent="0.3">
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="14" x14ac:dyDescent="0.3">
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="14" x14ac:dyDescent="0.3">
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="14" x14ac:dyDescent="0.3">
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="14" x14ac:dyDescent="0.3">
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="14" x14ac:dyDescent="0.3">
-      <c r="A24" s="1"/>
-    </row>
-    <row r="25" spans="1:1" ht="14" x14ac:dyDescent="0.3">
-      <c r="A25" s="1"/>
-    </row>
-    <row r="26" spans="1:1" ht="14" x14ac:dyDescent="0.3">
-      <c r="A26" s="1"/>
-    </row>
-    <row r="27" spans="1:1" ht="14" x14ac:dyDescent="0.3">
-      <c r="A27" s="1"/>
-    </row>
-    <row r="28" spans="1:1" ht="14" x14ac:dyDescent="0.3">
-      <c r="A28" s="1"/>
-    </row>
-    <row r="29" spans="1:1" ht="14" x14ac:dyDescent="0.3">
-      <c r="A29" s="1"/>
-    </row>
-    <row r="30" spans="1:1" ht="14" x14ac:dyDescent="0.3">
-      <c r="A30" s="1"/>
-    </row>
-    <row r="31" spans="1:1" ht="14" x14ac:dyDescent="0.3">
-      <c r="A31" s="1"/>
-    </row>
-    <row r="32" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="2"/>
-    </row>
-    <row r="33" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="2"/>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>